<commit_message>
Everthing works fine in IE,but occupance breaks for Chrome
</commit_message>
<xml_diff>
--- a/src/test/java/Utils/Testdata.xlsx
+++ b/src/test/java/Utils/Testdata.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14655" windowHeight="7500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14655" windowHeight="7500" firstSheet="10" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="263">
   <si>
     <t>username</t>
   </si>
@@ -635,202 +635,202 @@
     <t>Maddress 1</t>
   </si>
   <si>
+    <t>9/15/2017</t>
+  </si>
+  <si>
+    <t>Effectivedate</t>
+  </si>
+  <si>
+    <t>Expected HO Premium</t>
+  </si>
+  <si>
+    <t>Expected HOB Premium</t>
+  </si>
+  <si>
+    <t>Actual HO Premium</t>
+  </si>
+  <si>
+    <t>Actual HOB Premium</t>
+  </si>
+  <si>
+    <t>Pass/Fail</t>
+  </si>
+  <si>
+    <t>1244</t>
+  </si>
+  <si>
+    <t>1055</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>HOA</t>
+  </si>
+  <si>
+    <t>Houma</t>
+  </si>
+  <si>
+    <t>70360</t>
+  </si>
+  <si>
+    <t>501 July dr</t>
+  </si>
+  <si>
+    <t>Fin</t>
+  </si>
+  <si>
+    <t>Lam</t>
+  </si>
+  <si>
+    <t>12/10/1978</t>
+  </si>
+  <si>
+    <t>2011</t>
+  </si>
+  <si>
+    <t>1989</t>
+  </si>
+  <si>
+    <t>9/12/2015</t>
+  </si>
+  <si>
+    <t>250000</t>
+  </si>
+  <si>
+    <t>Masonry</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>500,000</t>
+  </si>
+  <si>
+    <t>$3,000</t>
+  </si>
+  <si>
+    <t>25%</t>
+  </si>
+  <si>
+    <t>2%</t>
+  </si>
+  <si>
+    <t>HOANAme</t>
+  </si>
+  <si>
+    <t>1202</t>
+  </si>
+  <si>
+    <t>77897</t>
+  </si>
+  <si>
+    <t>Corp</t>
+  </si>
+  <si>
+    <t>1442</t>
+  </si>
+  <si>
+    <t>1192</t>
+  </si>
+  <si>
+    <t>Professional Appr</t>
+  </si>
+  <si>
+    <t>Stilts with Sweep Away Walls</t>
+  </si>
+  <si>
+    <t>Built Up Or Hot Mopped Without Gravel</t>
+  </si>
+  <si>
+    <t>Single-Family</t>
+  </si>
+  <si>
+    <t>2191</t>
+  </si>
+  <si>
+    <t>1707</t>
+  </si>
+  <si>
+    <t>Raddress2</t>
+  </si>
+  <si>
+    <t>ksasidha@hotmail.com</t>
+  </si>
+  <si>
+    <t>PrimaryAgent</t>
+  </si>
+  <si>
+    <t>Primary2 Agent2</t>
+  </si>
+  <si>
+    <t>contact</t>
+  </si>
+  <si>
+    <t>1212121212</t>
+  </si>
+  <si>
+    <t>kripasasidharan@hotmail.com</t>
+  </si>
+  <si>
+    <t>EarthQuake</t>
+  </si>
+  <si>
+    <t>EQ Deductible</t>
+  </si>
+  <si>
+    <t>HighRisk</t>
+  </si>
+  <si>
+    <t>MasonaryChimney</t>
+  </si>
+  <si>
+    <t>Cripplestud</t>
+  </si>
+  <si>
+    <t>Construction material</t>
+  </si>
+  <si>
+    <t>Cliff</t>
+  </si>
+  <si>
+    <t>SolidGround</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>slope</t>
+  </si>
+  <si>
     <t>3</t>
   </si>
   <si>
-    <t>9/15/2017</t>
-  </si>
-  <si>
-    <t>Effectivedate</t>
-  </si>
-  <si>
-    <t>Expected HO Premium</t>
-  </si>
-  <si>
-    <t>Expected HOB Premium</t>
-  </si>
-  <si>
-    <t>Actual HO Premium</t>
-  </si>
-  <si>
-    <t>Actual HOB Premium</t>
-  </si>
-  <si>
-    <t>Pass/Fail</t>
-  </si>
-  <si>
-    <t>1244</t>
-  </si>
-  <si>
-    <t>1055</t>
-  </si>
-  <si>
-    <t>Fail</t>
-  </si>
-  <si>
-    <t>HOA</t>
-  </si>
-  <si>
-    <t>Houma</t>
-  </si>
-  <si>
-    <t>70360</t>
-  </si>
-  <si>
-    <t>501 July dr</t>
-  </si>
-  <si>
-    <t>Fin</t>
-  </si>
-  <si>
-    <t>Lam</t>
-  </si>
-  <si>
-    <t>12/10/1978</t>
-  </si>
-  <si>
-    <t>2011</t>
-  </si>
-  <si>
-    <t>1989</t>
-  </si>
-  <si>
-    <t>9/12/2015</t>
-  </si>
-  <si>
-    <t>250000</t>
-  </si>
-  <si>
-    <t>Masonry</t>
-  </si>
-  <si>
-    <t>1.0</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>Owner</t>
-  </si>
-  <si>
-    <t>500,000</t>
-  </si>
-  <si>
-    <t>$3,000</t>
-  </si>
-  <si>
-    <t>25%</t>
-  </si>
-  <si>
-    <t>2%</t>
-  </si>
-  <si>
-    <t>HOANAme</t>
-  </si>
-  <si>
-    <t>1202</t>
-  </si>
-  <si>
-    <t>77897</t>
-  </si>
-  <si>
-    <t>Corp</t>
-  </si>
-  <si>
-    <t>1442</t>
-  </si>
-  <si>
-    <t>1192</t>
-  </si>
-  <si>
-    <t>Professional Appr</t>
-  </si>
-  <si>
-    <t>Stilts with Sweep Away Walls</t>
-  </si>
-  <si>
-    <t>Built Up Or Hot Mopped Without Gravel</t>
-  </si>
-  <si>
-    <t>Single-Family</t>
-  </si>
-  <si>
-    <t>2191</t>
-  </si>
-  <si>
-    <t>1707</t>
-  </si>
-  <si>
-    <t>Raddress2</t>
-  </si>
-  <si>
-    <t>ksasidha@hotmail.com</t>
-  </si>
-  <si>
-    <t>PrimaryAgent</t>
-  </si>
-  <si>
-    <t>Primary2 Agent2</t>
-  </si>
-  <si>
-    <t>contact</t>
-  </si>
-  <si>
-    <t>1212121212</t>
-  </si>
-  <si>
-    <t>kripasasidharan@hotmail.com</t>
-  </si>
-  <si>
-    <t>EarthQuake</t>
-  </si>
-  <si>
-    <t>EQ Deductible</t>
-  </si>
-  <si>
-    <t>HighRisk</t>
-  </si>
-  <si>
-    <t>MasonaryChimney</t>
-  </si>
-  <si>
-    <t>Cripplestud</t>
-  </si>
-  <si>
-    <t>Construction material</t>
-  </si>
-  <si>
-    <t>Cliff</t>
-  </si>
-  <si>
-    <t>SolidGround</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>slope</t>
-  </si>
-  <si>
-    <t>108 E Walnut Cir</t>
-  </si>
-  <si>
-    <t>Summerville</t>
-  </si>
-  <si>
-    <t>29485</t>
-  </si>
-  <si>
-    <t>SC</t>
-  </si>
-  <si>
-    <t>Jeff </t>
-  </si>
-  <si>
-    <t>Bowers </t>
+    <t>MISTY</t>
+  </si>
+  <si>
+    <t>LOPAZ</t>
+  </si>
+  <si>
+    <t>808 Transcontinental Dr</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Metairie</t>
+  </si>
+  <si>
+    <t>70002</t>
   </si>
 </sst>
 </file>
@@ -840,7 +840,7 @@
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -872,6 +872,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -893,7 +900,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -917,6 +924,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1254,23 +1262,23 @@
         <v>1</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>2</v>
@@ -1336,7 +1344,7 @@
         <v>83</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C3" t="s">
         <v>83</v>
@@ -1354,8 +1362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1446,7 +1454,7 @@
         <v>83</v>
       </c>
       <c r="M2" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="N2" t="s">
         <v>17</v>
@@ -1454,7 +1462,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>92</v>
@@ -1463,10 +1471,10 @@
         <v>89</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="E3" t="s">
         <v>222</v>
-      </c>
-      <c r="E3" t="s">
-        <v>223</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>92</v>
@@ -1506,7 +1514,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1588,7 +1596,7 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B1" t="s">
         <v>164</v>
@@ -1658,7 +1666,7 @@
         <v>174</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="R2" s="7">
         <v>2000</v>
@@ -1670,28 +1678,28 @@
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H3" s="8" t="s">
+      <c r="I3" s="8" t="s">
         <v>226</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>227</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>175</v>
@@ -1817,31 +1825,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B1" t="s">
         <v>247</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>248</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>249</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>250</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>251</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>255</v>
+      </c>
+      <c r="H1" t="s">
         <v>252</v>
       </c>
-      <c r="G1" t="s">
-        <v>256</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>253</v>
-      </c>
-      <c r="I1" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1855,22 +1863,22 @@
         <v>83</v>
       </c>
       <c r="D2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -1883,7 +1891,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1929,7 +1937,7 @@
         <v>83</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>197</v>
+        <v>256</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2027,7 +2035,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>92</v>
@@ -2036,13 +2044,13 @@
         <v>92</v>
       </c>
       <c r="D3" t="s">
+        <v>227</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>228</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>229</v>
       </c>
       <c r="G3" t="s">
         <v>191</v>
@@ -2051,7 +2059,7 @@
         <v>192</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -2129,7 +2137,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>92</v>
@@ -2144,7 +2152,7 @@
         <v>188</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G3" t="s">
         <v>191</v>
@@ -2153,7 +2161,7 @@
         <v>192</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -2203,7 +2211,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B2" t="s">
         <v>185</v>
@@ -2265,36 +2273,36 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B1" t="s">
         <v>200</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>201</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>202</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>203</v>
-      </c>
-      <c r="E1" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>205</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="C2" t="s">
+        <v>231</v>
+      </c>
+      <c r="D2" t="s">
+        <v>232</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>206</v>
-      </c>
-      <c r="C2" t="s">
-        <v>232</v>
-      </c>
-      <c r="D2" t="s">
-        <v>233</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2305,10 +2313,10 @@
         <v>92</v>
       </c>
       <c r="C3" t="s">
+        <v>237</v>
+      </c>
+      <c r="D3" t="s">
         <v>238</v>
-      </c>
-      <c r="D3" t="s">
-        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -2321,7 +2329,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J2" sqref="J2:N2"/>
     </sheetView>
   </sheetViews>
@@ -2387,48 +2395,52 @@
         <v>22</v>
       </c>
       <c r="O1" s="13" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="17" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="21" t="s">
-        <v>261</v>
+      <c r="A2" s="23" t="s">
+        <v>257</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C2" s="15"/>
       <c r="D2" s="16">
         <v>28834</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="F2" s="14"/>
+        <v>259</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>260</v>
+      </c>
       <c r="G2" s="3" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="H2" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="I2" s="22" t="s">
+        <v>262</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="K2" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="I2" s="22" t="s">
-        <v>259</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="K2" s="14"/>
       <c r="L2" s="3" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="M2" s="17" t="s">
-        <v>260</v>
+        <v>108</v>
       </c>
       <c r="N2" s="22" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="O2" s="19" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -2519,13 +2531,13 @@
         <v>83</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="5" t="s">
         <v>213</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>214</v>
       </c>
       <c r="E3" t="s">
         <v>26</v>
@@ -2554,7 +2566,7 @@
   <dimension ref="A1:N40"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2577,7 +2589,7 @@
         <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C1" t="s">
         <v>30</v>
@@ -2615,36 +2627,40 @@
     </row>
     <row r="2" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="B2" s="2"/>
+        <v>259</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>260</v>
+      </c>
       <c r="C2" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="D2" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>262</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="G2" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="G2" s="2"/>
       <c r="H2" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>260</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>259</v>
+        <v>261</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="J2" s="22" t="s">
+        <v>262</v>
       </c>
       <c r="K2" t="s">
         <v>76</v>
       </c>
       <c r="L2" t="s">
-        <v>71</v>
+        <v>44</v>
       </c>
       <c r="N2" t="s">
         <v>37</v>
@@ -2652,30 +2668,30 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>108</v>
       </c>
       <c r="E3" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>210</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>211</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>108</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>76</v>
@@ -3070,13 +3086,13 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>215</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>216</v>
       </c>
       <c r="D3" t="s">
         <v>17</v>
@@ -3085,19 +3101,19 @@
         <v>17</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" t="s">
+        <v>233</v>
+      </c>
+      <c r="I3" t="s">
         <v>218</v>
       </c>
-      <c r="H3" t="s">
-        <v>234</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="J3" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>220</v>
       </c>
       <c r="K3" t="s">
         <v>17</v>
@@ -3182,10 +3198,10 @@
         <v>92</v>
       </c>
       <c r="C3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E3" t="s">
         <v>17</v>

</xml_diff>